<commit_message>
update Revisi Anggaran 18 Januari 2023
</commit_message>
<xml_diff>
--- a/Revisi Anggaran/Revisi Anggaran 1/Revisi MK 2023.xlsx
+++ b/Revisi Anggaran/Revisi Anggaran 1/Revisi MK 2023.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BACK\PUSDIK\2023\Github\TA.2023\Revisi Anggaran\Revisi Anggaran 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F07D92-D4D1-4EBA-9E81-63CCA08B24F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA58B1AB-77D4-4473-8105-FFD895B51D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{565EA5FA-1DAB-427E-93A3-16D88B5F5D47}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{565EA5FA-1DAB-427E-93A3-16D88B5F5D47}"/>
   </bookViews>
   <sheets>
     <sheet name="USULAN REVISI" sheetId="1" r:id="rId1"/>
     <sheet name="Perjalanan Pusdik" sheetId="2" r:id="rId2"/>
     <sheet name="Fullboard" sheetId="4" r:id="rId3"/>
+    <sheet name="Fullboard_Revisi" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Fullboard!$A$1:$N$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">Fullboard_Revisi!$A$1:$N$23</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Perjalanan Pusdik'!$A$1:$M$19</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'USULAN REVISI'!$A$1:$M$74</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'USULAN REVISI'!$5:$10</definedName>
@@ -31,9 +33,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="99">
   <si>
     <t>SUB KOORDINATOR KELOMPOK METODE DAN KURIKULUM</t>
   </si>
@@ -1009,6 +1014,24 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1042,23 +1065,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1080,15 +1094,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1466,7 +1471,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1476,195 +1481,195 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FD0258F-BBF2-4E29-BA1E-8CC0129EFF16}">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="56.109375" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" style="13" customWidth="1"/>
     <col min="4" max="4" width="6" style="13" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" style="13" customWidth="1"/>
     <col min="6" max="6" width="14" style="13" customWidth="1"/>
-    <col min="7" max="7" width="1.140625" style="14" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="52.140625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="1.109375" style="14" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" style="13" customWidth="1"/>
+    <col min="9" max="9" width="52.109375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="8.44140625" style="13" customWidth="1"/>
     <col min="11" max="11" width="7" style="13" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="13" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" style="13" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="22.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="108" t="s">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="114" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
-      <c r="F1" s="108"/>
-      <c r="G1" s="108"/>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="108"/>
-      <c r="M1" s="108"/>
-    </row>
-    <row r="2" spans="1:13" ht="22.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="108" t="s">
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+    </row>
+    <row r="2" spans="1:13" ht="21" x14ac:dyDescent="0.5">
+      <c r="A2" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
-      <c r="E2" s="108"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="108"/>
-      <c r="M2" s="108"/>
-    </row>
-    <row r="3" spans="1:13" ht="22.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="109"/>
-      <c r="B3" s="110"/>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="110"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="110"/>
-      <c r="K3" s="110"/>
-      <c r="L3" s="110"/>
-      <c r="M3" s="110"/>
-    </row>
-    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="111"/>
-      <c r="B4" s="111"/>
-      <c r="C4" s="111"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="111"/>
-      <c r="F4" s="111"/>
-      <c r="G4" s="111"/>
-      <c r="H4" s="111"/>
-      <c r="I4" s="111"/>
-      <c r="J4" s="111"/>
-      <c r="K4" s="111"/>
-      <c r="L4" s="111"/>
-      <c r="M4" s="111"/>
-    </row>
-    <row r="5" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="112" t="s">
+      <c r="B2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="114"/>
+      <c r="M2" s="114"/>
+    </row>
+    <row r="3" spans="1:13" ht="21" x14ac:dyDescent="0.5">
+      <c r="A3" s="115"/>
+      <c r="B3" s="116"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="116"/>
+      <c r="G3" s="116"/>
+      <c r="H3" s="116"/>
+      <c r="I3" s="116"/>
+      <c r="J3" s="116"/>
+      <c r="K3" s="116"/>
+      <c r="L3" s="116"/>
+      <c r="M3" s="116"/>
+    </row>
+    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="117"/>
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="117"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="117"/>
+      <c r="H4" s="117"/>
+      <c r="I4" s="117"/>
+      <c r="J4" s="117"/>
+      <c r="K4" s="117"/>
+      <c r="L4" s="117"/>
+      <c r="M4" s="117"/>
+    </row>
+    <row r="5" spans="1:13" ht="25.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="113"/>
-      <c r="C5" s="113"/>
-      <c r="D5" s="113"/>
-      <c r="E5" s="113"/>
-      <c r="F5" s="114"/>
+      <c r="B5" s="119"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="119"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="120"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="118" t="s">
+      <c r="H5" s="124" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="118"/>
-      <c r="J5" s="118"/>
-      <c r="K5" s="118"/>
-      <c r="L5" s="118"/>
-      <c r="M5" s="118"/>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="115"/>
-      <c r="B6" s="116"/>
-      <c r="C6" s="116"/>
-      <c r="D6" s="116"/>
-      <c r="E6" s="116"/>
-      <c r="F6" s="117"/>
+      <c r="I5" s="124"/>
+      <c r="J5" s="124"/>
+      <c r="K5" s="124"/>
+      <c r="L5" s="124"/>
+      <c r="M5" s="124"/>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="121"/>
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="123"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="118"/>
-      <c r="I6" s="118"/>
-      <c r="J6" s="118"/>
-      <c r="K6" s="118"/>
-      <c r="L6" s="118"/>
-      <c r="M6" s="118"/>
-    </row>
-    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="121" t="s">
+      <c r="H6" s="124"/>
+      <c r="I6" s="124"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="124"/>
+      <c r="M6" s="124"/>
+    </row>
+    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="121" t="s">
+      <c r="B7" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="123" t="s">
+      <c r="C7" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="119" t="s">
+      <c r="D7" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="119" t="s">
+      <c r="E7" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="119" t="s">
+      <c r="F7" s="108" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="121" t="s">
+      <c r="H7" s="110" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="121" t="s">
+      <c r="I7" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="123" t="s">
+      <c r="J7" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="119" t="s">
+      <c r="K7" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="119" t="s">
+      <c r="L7" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="119" t="s">
+      <c r="M7" s="108" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="121"/>
-      <c r="B8" s="121"/>
-      <c r="C8" s="123"/>
-      <c r="D8" s="119"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="119"/>
+    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="110"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="112"/>
+      <c r="D8" s="108"/>
+      <c r="E8" s="108"/>
+      <c r="F8" s="108"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="121"/>
-      <c r="I8" s="121"/>
-      <c r="J8" s="123"/>
-      <c r="K8" s="119"/>
-      <c r="L8" s="119"/>
-      <c r="M8" s="119"/>
-    </row>
-    <row r="9" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="122"/>
-      <c r="B9" s="122"/>
-      <c r="C9" s="124"/>
-      <c r="D9" s="120"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
+      <c r="H8" s="110"/>
+      <c r="I8" s="110"/>
+      <c r="J8" s="112"/>
+      <c r="K8" s="108"/>
+      <c r="L8" s="108"/>
+      <c r="M8" s="108"/>
+    </row>
+    <row r="9" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="111"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="113"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="122"/>
-      <c r="I9" s="122"/>
-      <c r="J9" s="124"/>
-      <c r="K9" s="120"/>
-      <c r="L9" s="120"/>
-      <c r="M9" s="120"/>
-    </row>
-    <row r="10" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="111"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="113"/>
+      <c r="K9" s="109"/>
+      <c r="L9" s="109"/>
+      <c r="M9" s="109"/>
+    </row>
+    <row r="10" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1703,7 +1708,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="23"/>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -1724,7 +1729,7 @@
         <v>651753000</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="6" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="95" t="s">
         <v>78</v>
       </c>
@@ -1753,7 +1758,7 @@
         <v>243442000</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="74">
         <v>521211</v>
       </c>
@@ -1782,7 +1787,7 @@
         <v>48225000</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="78"/>
       <c r="B14" s="79" t="s">
         <v>30</v>
@@ -1820,7 +1825,7 @@
         <v>39975000</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="78"/>
       <c r="B15" s="79" t="s">
         <v>31</v>
@@ -1857,7 +1862,7 @@
         <v>750000</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="78"/>
       <c r="B16" s="79" t="s">
         <v>33</v>
@@ -1894,7 +1899,7 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="78"/>
       <c r="B17" s="79" t="s">
         <v>34</v>
@@ -1931,7 +1936,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="74">
         <v>522151</v>
       </c>
@@ -1960,7 +1965,7 @@
         <v>16000000</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="78"/>
       <c r="B19" s="79" t="s">
         <v>35</v>
@@ -1997,7 +2002,7 @@
         <v>16000000</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="74">
         <v>524111</v>
       </c>
@@ -2026,7 +2031,7 @@
         <v>67448000</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="19" t="s">
         <v>36</v>
@@ -2064,7 +2069,7 @@
         <v>67448000</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
       <c r="B22" s="19"/>
       <c r="C22" s="20"/>
@@ -2084,7 +2089,7 @@
         <v>111769000</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
       <c r="B23" s="19"/>
       <c r="C23" s="20"/>
@@ -2111,7 +2116,7 @@
         <v>83790000</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18"/>
       <c r="B24" s="19"/>
       <c r="C24" s="20"/>
@@ -2139,7 +2144,7 @@
         <v>27979000</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A25" s="95" t="s">
         <v>79</v>
       </c>
@@ -2168,7 +2173,7 @@
         <v>54519000</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="74">
         <v>521211</v>
       </c>
@@ -2197,7 +2202,7 @@
         <v>17550000</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="78"/>
       <c r="B27" s="79" t="s">
         <v>30</v>
@@ -2235,7 +2240,7 @@
         <v>9300000</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="78"/>
       <c r="B28" s="79" t="s">
         <v>31</v>
@@ -2272,7 +2277,7 @@
         <v>750000</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="78"/>
       <c r="B29" s="79" t="s">
         <v>33</v>
@@ -2309,7 +2314,7 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="78"/>
       <c r="B30" s="79" t="s">
         <v>34</v>
@@ -2346,7 +2351,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="74">
         <v>522151</v>
       </c>
@@ -2375,7 +2380,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="78"/>
       <c r="B32" s="79" t="s">
         <v>35</v>
@@ -2412,7 +2417,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="74">
         <v>524111</v>
       </c>
@@ -2441,7 +2446,7 @@
         <v>31969000</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="78"/>
       <c r="B34" s="79" t="s">
         <v>37</v>
@@ -2479,7 +2484,7 @@
         <v>31969000</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A35" s="96" t="s">
         <v>77</v>
       </c>
@@ -2508,7 +2513,7 @@
         <v>99334000</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="25" t="s">
         <v>42</v>
       </c>
@@ -2537,7 +2542,7 @@
         <v>24800000</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="28"/>
       <c r="B37" s="29" t="s">
         <v>30</v>
@@ -2575,7 +2580,7 @@
         <v>19050000</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="28"/>
       <c r="B38" s="29" t="s">
         <v>31</v>
@@ -2612,7 +2617,7 @@
         <v>750000</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="28"/>
       <c r="B39" s="29" t="s">
         <v>33</v>
@@ -2649,7 +2654,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="28"/>
       <c r="B40" s="29" t="s">
         <v>34</v>
@@ -2686,7 +2691,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="31" t="s">
         <v>43</v>
       </c>
@@ -2715,7 +2720,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="28"/>
       <c r="B42" s="29" t="s">
         <v>44</v>
@@ -2752,7 +2757,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="25" t="s">
         <v>45</v>
       </c>
@@ -2781,7 +2786,7 @@
         <v>71534000</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A44" s="28"/>
       <c r="B44" s="29" t="s">
         <v>46</v>
@@ -2819,7 +2824,7 @@
         <v>71534000</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" s="6" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A45" s="95" t="s">
         <v>76</v>
       </c>
@@ -2848,7 +2853,7 @@
         <v>78803000</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="74">
         <v>521211</v>
       </c>
@@ -2877,7 +2882,7 @@
         <v>15500000</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="78"/>
       <c r="B47" s="79" t="s">
         <v>30</v>
@@ -2915,7 +2920,7 @@
         <v>9750000</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="78"/>
       <c r="B48" s="79" t="s">
         <v>39</v>
@@ -2952,7 +2957,7 @@
         <v>750000</v>
       </c>
     </row>
-    <row r="49" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="78"/>
       <c r="B49" s="79" t="s">
         <v>33</v>
@@ -2989,7 +2994,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="50" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="78"/>
       <c r="B50" s="79" t="s">
         <v>34</v>
@@ -3026,7 +3031,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="74">
         <v>522151</v>
       </c>
@@ -3055,7 +3060,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="52" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="78"/>
       <c r="B52" s="79" t="s">
         <v>35</v>
@@ -3092,7 +3097,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="53" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="74">
         <v>524111</v>
       </c>
@@ -3121,7 +3126,7 @@
         <v>43303000</v>
       </c>
     </row>
-    <row r="54" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="78"/>
       <c r="B54" s="79" t="s">
         <v>40</v>
@@ -3159,7 +3164,7 @@
         <v>43303000</v>
       </c>
     </row>
-    <row r="55" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="102"/>
       <c r="B55" s="103"/>
       <c r="C55" s="102"/>
@@ -3179,7 +3184,7 @@
         <v>175655000</v>
       </c>
     </row>
-    <row r="56" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="74"/>
       <c r="B56" s="75"/>
       <c r="C56" s="74"/>
@@ -3201,7 +3206,7 @@
         <v>11000000</v>
       </c>
     </row>
-    <row r="57" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="78"/>
       <c r="B57" s="79"/>
       <c r="C57" s="78"/>
@@ -3227,7 +3232,7 @@
         <v>7500000</v>
       </c>
     </row>
-    <row r="58" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="78"/>
       <c r="B58" s="79"/>
       <c r="C58" s="78"/>
@@ -3253,7 +3258,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="59" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="78"/>
       <c r="B59" s="79"/>
       <c r="C59" s="78"/>
@@ -3279,7 +3284,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="60" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="78"/>
       <c r="B60" s="79"/>
       <c r="C60" s="78"/>
@@ -3305,7 +3310,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="61" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="74"/>
       <c r="B61" s="75"/>
       <c r="C61" s="74"/>
@@ -3327,7 +3332,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="62" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="78"/>
       <c r="B62" s="79"/>
       <c r="C62" s="78"/>
@@ -3353,7 +3358,7 @@
         <v>20000000</v>
       </c>
     </row>
-    <row r="63" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="74"/>
       <c r="B63" s="75"/>
       <c r="C63" s="74"/>
@@ -3375,7 +3380,7 @@
         <v>144655000</v>
       </c>
     </row>
-    <row r="64" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="78"/>
       <c r="B64" s="79"/>
       <c r="C64" s="78"/>
@@ -3403,7 +3408,7 @@
         <v>144655000</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="7"/>
       <c r="B65" s="10"/>
       <c r="C65" s="8"/>
@@ -3418,7 +3423,7 @@
       <c r="L65" s="8"/>
       <c r="M65" s="11"/>
     </row>
-    <row r="66" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="7"/>
       <c r="B66" s="10"/>
       <c r="C66" s="8"/>
@@ -3433,7 +3438,7 @@
       <c r="L66" s="8"/>
       <c r="M66" s="11"/>
     </row>
-    <row r="67" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="7"/>
       <c r="B67" s="10"/>
       <c r="C67" s="8"/>
@@ -3450,7 +3455,7 @@
       <c r="L67" s="8"/>
       <c r="M67" s="11"/>
     </row>
-    <row r="68" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="7"/>
       <c r="B68" s="105" t="s">
         <v>94</v>
@@ -3469,7 +3474,7 @@
       <c r="L68" s="8"/>
       <c r="M68" s="11"/>
     </row>
-    <row r="69" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="7"/>
       <c r="B69" s="105" t="s">
         <v>95</v>
@@ -3487,7 +3492,7 @@
       <c r="L69" s="8"/>
       <c r="M69" s="11"/>
     </row>
-    <row r="70" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="7"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
@@ -3500,7 +3505,7 @@
       <c r="L70" s="8"/>
       <c r="M70" s="11"/>
     </row>
-    <row r="71" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="7"/>
       <c r="B71" s="10"/>
       <c r="C71" s="8"/>
@@ -3514,7 +3519,7 @@
       <c r="L71" s="8"/>
       <c r="M71" s="8"/>
     </row>
-    <row r="72" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="7"/>
       <c r="B72" s="10"/>
       <c r="C72" s="8"/>
@@ -3528,7 +3533,7 @@
       <c r="L72" s="8"/>
       <c r="M72" s="8"/>
     </row>
-    <row r="73" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="7"/>
       <c r="B73" s="12" t="s">
         <v>25</v>
@@ -3544,7 +3549,7 @@
       <c r="K73" s="8"/>
       <c r="M73" s="8"/>
     </row>
-    <row r="74" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="7"/>
       <c r="B74" s="10" t="s">
         <v>27</v>
@@ -3560,7 +3565,7 @@
       <c r="K74" s="8"/>
       <c r="M74" s="8"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="8"/>
@@ -3572,7 +3577,7 @@
       <c r="L75" s="8"/>
       <c r="M75" s="8"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="8"/>
@@ -3584,7 +3589,7 @@
       <c r="L76" s="8"/>
       <c r="M76" s="8"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="8"/>
@@ -3597,7 +3602,7 @@
       <c r="L77" s="8"/>
       <c r="M77" s="8"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="8"/>
@@ -3610,7 +3615,7 @@
       <c r="L78" s="8"/>
       <c r="M78" s="8"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="8"/>
@@ -3623,7 +3628,7 @@
       <c r="L79" s="8"/>
       <c r="M79" s="8"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="8"/>
@@ -3636,7 +3641,7 @@
       <c r="L80" s="8"/>
       <c r="M80" s="8"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="8"/>
@@ -3649,7 +3654,7 @@
       <c r="L81" s="8"/>
       <c r="M81" s="8"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="8"/>
@@ -3662,7 +3667,7 @@
       <c r="L82" s="8"/>
       <c r="M82" s="8"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="8"/>
@@ -3675,7 +3680,7 @@
       <c r="L83" s="8"/>
       <c r="M83" s="8"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="8"/>
@@ -3690,6 +3695,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A5:F6"/>
+    <mergeCell ref="H5:M6"/>
     <mergeCell ref="M7:M9"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:B9"/>
@@ -3702,12 +3713,6 @@
     <mergeCell ref="J7:J9"/>
     <mergeCell ref="K7:K9"/>
     <mergeCell ref="L7:L9"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A5:F6"/>
-    <mergeCell ref="H5:M6"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="A14:A17 H14:H17" xr:uid="{B48B5047-8C1F-4FFB-9FFA-F5906E31E514}">
@@ -3725,94 +3730,94 @@
   <dimension ref="A1:M76"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:M19"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="35" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" style="66" customWidth="1"/>
-    <col min="5" max="5" width="4.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="10.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" style="35" customWidth="1"/>
-    <col min="14" max="16384" width="9.28515625" style="73"/>
+    <col min="1" max="1" width="3.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" style="35" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" style="66" customWidth="1"/>
+    <col min="5" max="5" width="4.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="10.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" style="35" customWidth="1"/>
+    <col min="14" max="16384" width="9.33203125" style="73"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="132" t="s">
+    <row r="1" spans="1:13" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A1" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="132"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132"/>
-      <c r="L1" s="132"/>
-      <c r="M1" s="132"/>
-    </row>
-    <row r="2" spans="1:13" s="35" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="133" t="s">
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
+      <c r="M1" s="125"/>
+    </row>
+    <row r="2" spans="1:13" s="35" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="126" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="133"/>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="133"/>
-      <c r="H2" s="133"/>
-      <c r="I2" s="133"/>
-      <c r="J2" s="133"/>
-      <c r="K2" s="133"/>
-      <c r="L2" s="133"/>
-      <c r="M2" s="133"/>
-    </row>
-    <row r="3" spans="1:13" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="132" t="s">
+      <c r="B2" s="126"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="126"/>
+      <c r="G2" s="126"/>
+      <c r="H2" s="126"/>
+      <c r="I2" s="126"/>
+      <c r="J2" s="126"/>
+      <c r="K2" s="126"/>
+      <c r="L2" s="126"/>
+      <c r="M2" s="126"/>
+    </row>
+    <row r="3" spans="1:13" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="125" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="132"/>
-      <c r="J3" s="132"/>
-      <c r="K3" s="132"/>
-      <c r="L3" s="132"/>
-      <c r="M3" s="132"/>
-    </row>
-    <row r="4" spans="1:13" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="132" t="s">
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="125"/>
+      <c r="K3" s="125"/>
+      <c r="L3" s="125"/>
+      <c r="M3" s="125"/>
+    </row>
+    <row r="4" spans="1:13" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="125" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="132"/>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
-      <c r="H4" s="132"/>
-      <c r="I4" s="132"/>
-      <c r="J4" s="132"/>
-      <c r="K4" s="132"/>
-      <c r="L4" s="132"/>
-      <c r="M4" s="132"/>
-    </row>
-    <row r="5" spans="1:13" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4" s="125"/>
+      <c r="C4" s="125"/>
+      <c r="D4" s="125"/>
+      <c r="E4" s="125"/>
+      <c r="F4" s="125"/>
+      <c r="G4" s="125"/>
+      <c r="H4" s="125"/>
+      <c r="I4" s="125"/>
+      <c r="J4" s="125"/>
+      <c r="K4" s="125"/>
+      <c r="L4" s="125"/>
+      <c r="M4" s="125"/>
+    </row>
+    <row r="5" spans="1:13" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="34"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
@@ -3827,7 +3832,7 @@
       <c r="L5" s="34"/>
       <c r="M5" s="34"/>
     </row>
-    <row r="6" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="36"/>
       <c r="B6" s="37"/>
       <c r="C6" s="37"/>
@@ -3842,61 +3847,61 @@
       <c r="L6" s="40"/>
       <c r="M6" s="41"/>
     </row>
-    <row r="7" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="134" t="s">
+    <row r="7" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="127" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="134"/>
-      <c r="C7" s="134"/>
-      <c r="D7" s="134"/>
-      <c r="E7" s="134"/>
-      <c r="F7" s="134"/>
-      <c r="G7" s="134"/>
-      <c r="H7" s="134"/>
-      <c r="I7" s="134"/>
-      <c r="J7" s="134"/>
-      <c r="K7" s="134"/>
-      <c r="L7" s="134"/>
-      <c r="M7" s="134"/>
-    </row>
-    <row r="8" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="126" t="s">
+      <c r="B7" s="127"/>
+      <c r="C7" s="127"/>
+      <c r="D7" s="127"/>
+      <c r="E7" s="127"/>
+      <c r="F7" s="127"/>
+      <c r="G7" s="127"/>
+      <c r="H7" s="127"/>
+      <c r="I7" s="127"/>
+      <c r="J7" s="127"/>
+      <c r="K7" s="127"/>
+      <c r="L7" s="127"/>
+      <c r="M7" s="127"/>
+    </row>
+    <row r="8" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="129" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="126" t="s">
+      <c r="B8" s="129" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="126" t="s">
+      <c r="C8" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="130" t="s">
+      <c r="D8" s="133" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="125" t="s">
+      <c r="E8" s="128" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="125"/>
-      <c r="G8" s="125"/>
-      <c r="H8" s="125" t="s">
+      <c r="F8" s="128"/>
+      <c r="G8" s="128"/>
+      <c r="H8" s="128" t="s">
         <v>58</v>
       </c>
-      <c r="I8" s="125"/>
-      <c r="J8" s="125"/>
-      <c r="K8" s="126" t="s">
+      <c r="I8" s="128"/>
+      <c r="J8" s="128"/>
+      <c r="K8" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="L8" s="128" t="s">
+      <c r="L8" s="131" t="s">
         <v>60</v>
       </c>
-      <c r="M8" s="128" t="s">
+      <c r="M8" s="131" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="127"/>
-      <c r="B9" s="127"/>
-      <c r="C9" s="127"/>
-      <c r="D9" s="131"/>
+    <row r="9" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="130"/>
+      <c r="B9" s="130"/>
+      <c r="C9" s="130"/>
+      <c r="D9" s="134"/>
       <c r="E9" s="43" t="s">
         <v>62</v>
       </c>
@@ -3915,11 +3920,11 @@
       <c r="J9" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="127"/>
-      <c r="L9" s="128"/>
-      <c r="M9" s="128"/>
-    </row>
-    <row r="10" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K9" s="130"/>
+      <c r="L9" s="131"/>
+      <c r="M9" s="131"/>
+    </row>
+    <row r="10" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="46">
         <v>1</v>
       </c>
@@ -3961,7 +3966,7 @@
         <v>7410000</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="46">
         <v>2</v>
       </c>
@@ -4006,7 +4011,7 @@
         <v>24228000</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="46">
         <v>3</v>
       </c>
@@ -4051,7 +4056,7 @@
         <v>30013500</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="46">
         <v>4</v>
       </c>
@@ -4097,7 +4102,7 @@
         <v>23313000</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="46">
         <v>5</v>
       </c>
@@ -4139,7 +4144,7 @@
         <v>10086000</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="46">
         <v>6</v>
       </c>
@@ -4183,7 +4188,7 @@
         <v>20649000</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="46">
         <v>7</v>
       </c>
@@ -4228,7 +4233,7 @@
         <v>18390000</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="46">
         <v>8</v>
       </c>
@@ -4272,7 +4277,7 @@
         <v>10566000</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="46"/>
       <c r="B18" s="47"/>
       <c r="C18" s="47"/>
@@ -4293,27 +4298,27 @@
         <v>144655500</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="129" t="s">
+    <row r="19" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="132" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="129"/>
-      <c r="C19" s="129"/>
-      <c r="D19" s="129"/>
-      <c r="E19" s="129"/>
-      <c r="F19" s="129"/>
-      <c r="G19" s="129"/>
-      <c r="H19" s="129"/>
-      <c r="I19" s="129"/>
-      <c r="J19" s="129"/>
-      <c r="K19" s="129"/>
-      <c r="L19" s="129"/>
+      <c r="B19" s="132"/>
+      <c r="C19" s="132"/>
+      <c r="D19" s="132"/>
+      <c r="E19" s="132"/>
+      <c r="F19" s="132"/>
+      <c r="G19" s="132"/>
+      <c r="H19" s="132"/>
+      <c r="I19" s="132"/>
+      <c r="J19" s="132"/>
+      <c r="K19" s="132"/>
+      <c r="L19" s="132"/>
       <c r="M19" s="61">
         <f>M18/D18</f>
         <v>6027312.5</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="62"/>
       <c r="C20" s="62"/>
       <c r="D20" s="63"/>
@@ -4322,16 +4327,16 @@
       <c r="G20" s="64"/>
       <c r="M20" s="65"/>
     </row>
-    <row r="21" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="66"/>
       <c r="G21" s="67"/>
       <c r="M21" s="65"/>
     </row>
-    <row r="22" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="66"/>
       <c r="M22" s="65"/>
     </row>
-    <row r="23" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="68"/>
       <c r="C23" s="68"/>
       <c r="D23" s="69"/>
@@ -4342,7 +4347,7 @@
       <c r="L23" s="65"/>
       <c r="M23" s="65"/>
     </row>
-    <row r="24" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="68"/>
       <c r="C24" s="68"/>
       <c r="D24" s="69"/>
@@ -4352,16 +4357,16 @@
       <c r="K24" s="65"/>
       <c r="M24" s="65"/>
     </row>
-    <row r="25" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D25" s="66"/>
     </row>
-    <row r="26" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="66"/>
       <c r="E26" s="70"/>
       <c r="F26" s="70"/>
       <c r="G26" s="70"/>
     </row>
-    <row r="27" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="66"/>
       <c r="E27" s="70"/>
       <c r="F27" s="70"/>
@@ -4370,196 +4375,196 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="66"/>
       <c r="E28" s="70"/>
       <c r="F28" s="70"/>
       <c r="G28" s="70"/>
       <c r="J28" s="71"/>
     </row>
-    <row r="29" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D29" s="66"/>
       <c r="E29" s="70"/>
       <c r="F29" s="70"/>
       <c r="G29" s="70"/>
       <c r="J29" s="71"/>
     </row>
-    <row r="30" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D30" s="66"/>
       <c r="E30" s="70"/>
       <c r="F30" s="70"/>
       <c r="G30" s="70"/>
     </row>
-    <row r="31" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D31" s="66"/>
       <c r="E31" s="70"/>
       <c r="F31" s="70"/>
       <c r="G31" s="70"/>
     </row>
-    <row r="32" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D32" s="66"/>
       <c r="E32" s="70"/>
       <c r="F32" s="70"/>
       <c r="G32" s="70"/>
     </row>
-    <row r="33" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D33" s="66"/>
       <c r="E33" s="70"/>
       <c r="F33" s="70"/>
       <c r="G33" s="70"/>
     </row>
-    <row r="34" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D34" s="66"/>
       <c r="E34" s="70"/>
       <c r="F34" s="70"/>
       <c r="G34" s="70"/>
     </row>
-    <row r="35" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D35" s="66"/>
       <c r="E35" s="70"/>
       <c r="F35" s="70"/>
       <c r="G35" s="70"/>
       <c r="K35" s="68"/>
     </row>
-    <row r="36" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D36" s="66"/>
       <c r="E36" s="70"/>
       <c r="F36" s="70"/>
       <c r="G36" s="70"/>
     </row>
-    <row r="37" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D37" s="66"/>
       <c r="E37" s="70"/>
       <c r="F37" s="70"/>
       <c r="G37" s="70"/>
     </row>
-    <row r="38" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D38" s="66"/>
       <c r="E38" s="70"/>
       <c r="F38" s="70"/>
       <c r="G38" s="70"/>
     </row>
-    <row r="39" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D39" s="66"/>
       <c r="E39" s="70"/>
       <c r="F39" s="70"/>
       <c r="G39" s="70"/>
     </row>
-    <row r="40" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D40" s="66"/>
       <c r="E40" s="70"/>
       <c r="F40" s="70"/>
       <c r="G40" s="70"/>
     </row>
-    <row r="41" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D41" s="66"/>
       <c r="E41" s="70"/>
       <c r="F41" s="70"/>
       <c r="G41" s="70"/>
     </row>
-    <row r="42" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D42" s="66"/>
     </row>
-    <row r="43" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D43" s="66"/>
     </row>
-    <row r="44" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D44" s="66"/>
     </row>
-    <row r="45" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D45" s="66"/>
     </row>
-    <row r="46" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D46" s="66"/>
     </row>
-    <row r="47" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D47" s="66"/>
     </row>
-    <row r="48" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:11" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D48" s="66"/>
     </row>
-    <row r="49" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D49" s="66"/>
     </row>
-    <row r="50" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D50" s="66"/>
     </row>
-    <row r="51" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D51" s="66"/>
     </row>
-    <row r="52" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D52" s="66"/>
     </row>
-    <row r="53" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D53" s="66"/>
     </row>
-    <row r="54" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D54" s="66"/>
     </row>
-    <row r="55" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D55" s="66"/>
     </row>
-    <row r="56" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D56" s="66"/>
     </row>
-    <row r="57" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D57" s="66"/>
     </row>
-    <row r="58" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D58" s="66"/>
     </row>
-    <row r="59" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D59" s="66"/>
     </row>
-    <row r="60" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D60" s="66"/>
     </row>
-    <row r="61" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D61" s="66"/>
     </row>
-    <row r="62" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D62" s="66"/>
     </row>
-    <row r="63" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D63" s="66"/>
     </row>
-    <row r="64" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D64" s="66"/>
     </row>
-    <row r="65" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D65" s="66"/>
     </row>
-    <row r="66" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D66" s="66"/>
     </row>
-    <row r="67" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D67" s="66"/>
     </row>
-    <row r="68" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D68" s="66"/>
     </row>
-    <row r="69" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D69" s="66"/>
     </row>
-    <row r="70" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D70" s="66"/>
     </row>
-    <row r="71" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D71" s="66"/>
     </row>
-    <row r="72" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D72" s="66"/>
     </row>
-    <row r="73" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D73" s="66"/>
     </row>
-    <row r="74" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D74" s="66"/>
     </row>
-    <row r="75" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D75" s="66"/>
     </row>
-    <row r="76" spans="1:13" s="72" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="35"/>
       <c r="B76" s="35"/>
       <c r="C76" s="35"/>
@@ -4576,11 +4581,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A7:M7"/>
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="K8:K9"/>
     <mergeCell ref="L8:L9"/>
@@ -4591,6 +4591,11 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E8:G8"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A7:M7"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4602,81 +4607,81 @@
   <dimension ref="A1:N80"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9:N21"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="35" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" style="66" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="10.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" style="35" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.28515625" style="73"/>
+    <col min="1" max="1" width="3.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="35" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" style="35" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.88671875" style="66" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="10.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" style="35" customWidth="1"/>
+    <col min="12" max="12" width="4.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.33203125" style="73"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="35" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="133" t="s">
+    <row r="1" spans="1:14" s="35" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="126" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="133"/>
-      <c r="C1" s="133"/>
-      <c r="D1" s="133"/>
-      <c r="E1" s="133"/>
-      <c r="F1" s="133"/>
-      <c r="G1" s="133"/>
-      <c r="H1" s="133"/>
-      <c r="I1" s="133"/>
-      <c r="J1" s="133"/>
-      <c r="K1" s="133"/>
-      <c r="L1" s="133"/>
-      <c r="M1" s="133"/>
-      <c r="N1" s="133"/>
-    </row>
-    <row r="2" spans="1:14" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="132" t="s">
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="126"/>
+      <c r="L1" s="126"/>
+      <c r="M1" s="126"/>
+      <c r="N1" s="126"/>
+    </row>
+    <row r="2" spans="1:14" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="125" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="132"/>
-      <c r="C2" s="132"/>
-      <c r="D2" s="132"/>
-      <c r="E2" s="132"/>
-      <c r="F2" s="132"/>
-      <c r="G2" s="132"/>
-      <c r="H2" s="132"/>
-      <c r="I2" s="132"/>
-      <c r="J2" s="132"/>
-      <c r="K2" s="132"/>
-      <c r="L2" s="132"/>
-      <c r="M2" s="132"/>
-      <c r="N2" s="132"/>
-    </row>
-    <row r="3" spans="1:14" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="132" t="s">
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="125"/>
+      <c r="L2" s="125"/>
+      <c r="M2" s="125"/>
+      <c r="N2" s="125"/>
+    </row>
+    <row r="3" spans="1:14" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="125" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="132"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="132"/>
-      <c r="J3" s="132"/>
-      <c r="K3" s="132"/>
-      <c r="L3" s="132"/>
-      <c r="M3" s="132"/>
-      <c r="N3" s="132"/>
-    </row>
-    <row r="4" spans="1:14" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="125"/>
+      <c r="K3" s="125"/>
+      <c r="L3" s="125"/>
+      <c r="M3" s="125"/>
+      <c r="N3" s="125"/>
+    </row>
+    <row r="4" spans="1:14" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="34"/>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
@@ -4692,7 +4697,7 @@
       <c r="M4" s="34"/>
       <c r="N4" s="34"/>
     </row>
-    <row r="5" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="36"/>
       <c r="B5" s="36"/>
       <c r="C5" s="37"/>
@@ -4708,36 +4713,36 @@
       <c r="M5" s="39"/>
       <c r="N5" s="39"/>
     </row>
-    <row r="6" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="134"/>
-      <c r="B6" s="134"/>
-      <c r="C6" s="134"/>
-      <c r="D6" s="134"/>
-      <c r="E6" s="134"/>
-      <c r="F6" s="134"/>
-      <c r="G6" s="134"/>
-      <c r="H6" s="134"/>
-      <c r="I6" s="134"/>
-      <c r="J6" s="134"/>
-      <c r="K6" s="134"/>
-      <c r="L6" s="134"/>
-      <c r="M6" s="134"/>
-      <c r="N6" s="134"/>
-    </row>
-    <row r="7" spans="1:14" s="35" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="126" t="s">
+    <row r="6" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="127"/>
+      <c r="B6" s="127"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="127"/>
+      <c r="N6" s="127"/>
+    </row>
+    <row r="7" spans="1:14" s="35" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="129" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="126" t="s">
+      <c r="B7" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="126" t="s">
+      <c r="C7" s="129" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="126" t="s">
+      <c r="D7" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="130" t="s">
+      <c r="E7" s="133" t="s">
         <v>56</v>
       </c>
       <c r="F7" s="135" t="s">
@@ -4745,27 +4750,27 @@
       </c>
       <c r="G7" s="135"/>
       <c r="H7" s="135"/>
-      <c r="I7" s="126" t="s">
+      <c r="I7" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="J7" s="128" t="s">
+      <c r="J7" s="131" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="L7" s="125" t="s">
+      <c r="L7" s="128" t="s">
         <v>87</v>
       </c>
-      <c r="M7" s="125"/>
-      <c r="N7" s="125"/>
-    </row>
-    <row r="8" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="127"/>
-      <c r="B8" s="127"/>
-      <c r="C8" s="127"/>
-      <c r="D8" s="127"/>
-      <c r="E8" s="131"/>
+      <c r="M7" s="128"/>
+      <c r="N7" s="128"/>
+    </row>
+    <row r="8" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="130"/>
+      <c r="B8" s="130"/>
+      <c r="C8" s="130"/>
+      <c r="D8" s="130"/>
+      <c r="E8" s="134"/>
       <c r="F8" s="43" t="s">
         <v>62</v>
       </c>
@@ -4775,9 +4780,9 @@
       <c r="H8" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="127"/>
-      <c r="J8" s="128"/>
-      <c r="K8" s="128"/>
+      <c r="I8" s="130"/>
+      <c r="J8" s="131"/>
+      <c r="K8" s="131"/>
       <c r="L8" s="43" t="s">
         <v>62</v>
       </c>
@@ -4788,7 +4793,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="46">
         <v>1</v>
       </c>
@@ -4835,7 +4840,7 @@
         <v>2394000</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="46">
         <v>2</v>
       </c>
@@ -4880,7 +4885,7 @@
         <v>2394000</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="46">
         <v>3</v>
       </c>
@@ -4925,7 +4930,7 @@
         <v>2394000</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="46">
         <v>4</v>
       </c>
@@ -4970,7 +4975,7 @@
         <v>2394000</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="46">
         <v>5</v>
       </c>
@@ -5015,7 +5020,7 @@
         <v>2394000</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="46">
         <v>6</v>
       </c>
@@ -5060,7 +5065,7 @@
         <v>2394000</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="46">
         <v>7</v>
       </c>
@@ -5105,7 +5110,7 @@
         <v>2394000</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="46">
         <v>8</v>
       </c>
@@ -5148,7 +5153,7 @@
         <v>2394000</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="46">
         <v>9</v>
       </c>
@@ -5193,7 +5198,7 @@
         <v>11970000</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="46">
         <v>10</v>
       </c>
@@ -5238,7 +5243,7 @@
         <v>9576000</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="46">
         <v>11</v>
       </c>
@@ -5283,7 +5288,7 @@
         <v>19152000</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="46">
         <v>12</v>
       </c>
@@ -5328,7 +5333,7 @@
         <v>16758000</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="46">
         <v>13</v>
       </c>
@@ -5373,7 +5378,7 @@
         <v>7182000</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="46"/>
       <c r="B22" s="46"/>
       <c r="C22" s="47"/>
@@ -5398,7 +5403,7 @@
         <v>83790000</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="97" t="s">
         <v>71</v>
       </c>
@@ -5419,7 +5424,7 @@
       <c r="M23" s="97"/>
       <c r="N23" s="97"/>
     </row>
-    <row r="24" spans="1:14" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="C24" s="62"/>
       <c r="D24" s="62"/>
       <c r="E24" s="63"/>
@@ -5428,16 +5433,16 @@
       <c r="H24" s="64"/>
       <c r="K24" s="65"/>
     </row>
-    <row r="25" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E25" s="66"/>
       <c r="H25" s="67"/>
       <c r="K25" s="65"/>
     </row>
-    <row r="26" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E26" s="66"/>
       <c r="K26" s="65"/>
     </row>
-    <row r="27" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="68"/>
       <c r="D27" s="68"/>
       <c r="E27" s="69"/>
@@ -5448,7 +5453,7 @@
       <c r="J27" s="65"/>
       <c r="K27" s="65"/>
     </row>
-    <row r="28" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="68"/>
       <c r="D28" s="68"/>
       <c r="E28" s="69"/>
@@ -5458,16 +5463,16 @@
       <c r="I28" s="65"/>
       <c r="K28" s="65"/>
     </row>
-    <row r="29" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E29" s="66"/>
     </row>
-    <row r="30" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E30" s="66"/>
       <c r="F30" s="70"/>
       <c r="G30" s="70"/>
       <c r="H30" s="70"/>
     </row>
-    <row r="31" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E31" s="66"/>
       <c r="F31" s="70"/>
       <c r="G31" s="70"/>
@@ -5476,196 +5481,196 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E32" s="66"/>
       <c r="F32" s="70"/>
       <c r="G32" s="70"/>
       <c r="H32" s="70"/>
       <c r="N32" s="71"/>
     </row>
-    <row r="33" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E33" s="66"/>
       <c r="F33" s="70"/>
       <c r="G33" s="70"/>
       <c r="H33" s="70"/>
       <c r="N33" s="71"/>
     </row>
-    <row r="34" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E34" s="66"/>
       <c r="F34" s="70"/>
       <c r="G34" s="70"/>
       <c r="H34" s="70"/>
     </row>
-    <row r="35" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E35" s="66"/>
       <c r="F35" s="70"/>
       <c r="G35" s="70"/>
       <c r="H35" s="70"/>
     </row>
-    <row r="36" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E36" s="66"/>
       <c r="F36" s="70"/>
       <c r="G36" s="70"/>
       <c r="H36" s="70"/>
     </row>
-    <row r="37" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E37" s="66"/>
       <c r="F37" s="70"/>
       <c r="G37" s="70"/>
       <c r="H37" s="70"/>
     </row>
-    <row r="38" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E38" s="66"/>
       <c r="F38" s="70"/>
       <c r="G38" s="70"/>
       <c r="H38" s="70"/>
     </row>
-    <row r="39" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E39" s="66"/>
       <c r="F39" s="70"/>
       <c r="G39" s="70"/>
       <c r="H39" s="70"/>
       <c r="I39" s="68"/>
     </row>
-    <row r="40" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E40" s="66"/>
       <c r="F40" s="70"/>
       <c r="G40" s="70"/>
       <c r="H40" s="70"/>
     </row>
-    <row r="41" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E41" s="66"/>
       <c r="F41" s="70"/>
       <c r="G41" s="70"/>
       <c r="H41" s="70"/>
     </row>
-    <row r="42" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E42" s="66"/>
       <c r="F42" s="70"/>
       <c r="G42" s="70"/>
       <c r="H42" s="70"/>
     </row>
-    <row r="43" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E43" s="66"/>
       <c r="F43" s="70"/>
       <c r="G43" s="70"/>
       <c r="H43" s="70"/>
     </row>
-    <row r="44" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E44" s="66"/>
       <c r="F44" s="70"/>
       <c r="G44" s="70"/>
       <c r="H44" s="70"/>
     </row>
-    <row r="45" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E45" s="66"/>
       <c r="F45" s="70"/>
       <c r="G45" s="70"/>
       <c r="H45" s="70"/>
     </row>
-    <row r="46" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E46" s="66"/>
     </row>
-    <row r="47" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E47" s="66"/>
     </row>
-    <row r="48" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E48" s="66"/>
     </row>
-    <row r="49" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E49" s="66"/>
     </row>
-    <row r="50" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E50" s="66"/>
     </row>
-    <row r="51" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E51" s="66"/>
     </row>
-    <row r="52" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E52" s="66"/>
     </row>
-    <row r="53" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E53" s="66"/>
     </row>
-    <row r="54" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E54" s="66"/>
     </row>
-    <row r="55" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E55" s="66"/>
     </row>
-    <row r="56" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E56" s="66"/>
     </row>
-    <row r="57" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E57" s="66"/>
     </row>
-    <row r="58" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E58" s="66"/>
     </row>
-    <row r="59" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E59" s="66"/>
     </row>
-    <row r="60" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E60" s="66"/>
     </row>
-    <row r="61" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E61" s="66"/>
     </row>
-    <row r="62" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E62" s="66"/>
     </row>
-    <row r="63" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E63" s="66"/>
     </row>
-    <row r="64" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E64" s="66"/>
     </row>
-    <row r="65" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E65" s="66"/>
     </row>
-    <row r="66" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E66" s="66"/>
     </row>
-    <row r="67" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E67" s="66"/>
     </row>
-    <row r="68" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E68" s="66"/>
     </row>
-    <row r="69" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E69" s="66"/>
     </row>
-    <row r="70" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E70" s="66"/>
     </row>
-    <row r="71" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E71" s="66"/>
     </row>
-    <row r="72" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E72" s="66"/>
     </row>
-    <row r="73" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E73" s="66"/>
     </row>
-    <row r="74" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E74" s="66"/>
     </row>
-    <row r="75" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E75" s="66"/>
     </row>
-    <row r="76" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E76" s="66"/>
     </row>
-    <row r="77" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E77" s="66"/>
     </row>
-    <row r="78" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E78" s="66"/>
     </row>
-    <row r="79" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E79" s="66"/>
     </row>
-    <row r="80" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="35"/>
       <c r="B80" s="35"/>
       <c r="C80" s="35"/>
@@ -5701,4 +5706,1108 @@
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3715BA9C-136D-4215-AD45-E8BB3C5D49C3}">
+  <dimension ref="A1:N80"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="35" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" style="35" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.88671875" style="66" customWidth="1"/>
+    <col min="6" max="6" width="4.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="10.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" style="35" customWidth="1"/>
+    <col min="12" max="12" width="4.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.33203125" style="73"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="35" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="126" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="126"/>
+      <c r="L1" s="126"/>
+      <c r="M1" s="126"/>
+      <c r="N1" s="126"/>
+    </row>
+    <row r="2" spans="1:14" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="125" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="125"/>
+      <c r="L2" s="125"/>
+      <c r="M2" s="125"/>
+      <c r="N2" s="125"/>
+    </row>
+    <row r="3" spans="1:14" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="125" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="125"/>
+      <c r="K3" s="125"/>
+      <c r="L3" s="125"/>
+      <c r="M3" s="125"/>
+      <c r="N3" s="125"/>
+    </row>
+    <row r="4" spans="1:14" s="35" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+    </row>
+    <row r="5" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+    </row>
+    <row r="6" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="127"/>
+      <c r="B6" s="127"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="127"/>
+      <c r="N6" s="127"/>
+    </row>
+    <row r="7" spans="1:14" s="35" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="129" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="129" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="129" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="129" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="133" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="135" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="135"/>
+      <c r="H7" s="135"/>
+      <c r="I7" s="129" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="131" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" s="131" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="128" t="s">
+        <v>87</v>
+      </c>
+      <c r="M7" s="128"/>
+      <c r="N7" s="128"/>
+    </row>
+    <row r="8" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="130"/>
+      <c r="B8" s="130"/>
+      <c r="C8" s="130"/>
+      <c r="D8" s="130"/>
+      <c r="E8" s="134"/>
+      <c r="F8" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="130"/>
+      <c r="J8" s="131"/>
+      <c r="K8" s="131"/>
+      <c r="L8" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="M8" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="N8" s="43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="46">
+        <v>1</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="45">
+        <v>1</v>
+      </c>
+      <c r="F9" s="46">
+        <v>3</v>
+      </c>
+      <c r="G9" s="58">
+        <v>180000</v>
+      </c>
+      <c r="H9" s="53">
+        <f t="shared" ref="H9" si="0">F9*G9</f>
+        <v>540000</v>
+      </c>
+      <c r="I9" s="55">
+        <v>300000</v>
+      </c>
+      <c r="J9" s="59">
+        <v>3829000</v>
+      </c>
+      <c r="K9" s="52">
+        <f>(H9+I9+J9)*E9</f>
+        <v>4669000</v>
+      </c>
+      <c r="L9" s="46">
+        <v>2</v>
+      </c>
+      <c r="M9" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="N9" s="55">
+        <f>(L9*M9)*E9</f>
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="46">
+        <v>2</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="45">
+        <v>1</v>
+      </c>
+      <c r="F10" s="43">
+        <v>3</v>
+      </c>
+      <c r="G10" s="58">
+        <v>180000</v>
+      </c>
+      <c r="H10" s="49">
+        <f>G10*F10</f>
+        <v>540000</v>
+      </c>
+      <c r="I10" s="51">
+        <v>150000</v>
+      </c>
+      <c r="J10" s="44"/>
+      <c r="K10" s="52">
+        <f t="shared" ref="K10:K21" si="1">(H10+I10+J10)*E10</f>
+        <v>690000</v>
+      </c>
+      <c r="L10" s="43">
+        <v>2</v>
+      </c>
+      <c r="M10" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="N10" s="55">
+        <f t="shared" ref="N10:N21" si="2">(L10*M10)*E10</f>
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="46">
+        <v>3</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="45">
+        <v>1</v>
+      </c>
+      <c r="F11" s="46">
+        <v>3</v>
+      </c>
+      <c r="G11" s="58">
+        <v>180000</v>
+      </c>
+      <c r="H11" s="53">
+        <f t="shared" ref="H11:H21" si="3">F11*G11</f>
+        <v>540000</v>
+      </c>
+      <c r="I11" s="51">
+        <v>150000</v>
+      </c>
+      <c r="J11" s="59"/>
+      <c r="K11" s="52">
+        <f t="shared" si="1"/>
+        <v>690000</v>
+      </c>
+      <c r="L11" s="46">
+        <v>2</v>
+      </c>
+      <c r="M11" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="N11" s="55">
+        <f t="shared" si="2"/>
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="46">
+        <v>4</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="45">
+        <v>1</v>
+      </c>
+      <c r="F12" s="46">
+        <v>3</v>
+      </c>
+      <c r="G12" s="58">
+        <v>180000</v>
+      </c>
+      <c r="H12" s="53">
+        <f t="shared" si="3"/>
+        <v>540000</v>
+      </c>
+      <c r="I12" s="51">
+        <v>150000</v>
+      </c>
+      <c r="J12" s="56"/>
+      <c r="K12" s="52">
+        <f t="shared" si="1"/>
+        <v>690000</v>
+      </c>
+      <c r="L12" s="46">
+        <v>2</v>
+      </c>
+      <c r="M12" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="N12" s="55">
+        <f t="shared" si="2"/>
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="46">
+        <v>5</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="45">
+        <v>1</v>
+      </c>
+      <c r="F13" s="46">
+        <v>3</v>
+      </c>
+      <c r="G13" s="58">
+        <v>180000</v>
+      </c>
+      <c r="H13" s="53">
+        <f t="shared" si="3"/>
+        <v>540000</v>
+      </c>
+      <c r="I13" s="51">
+        <v>150000</v>
+      </c>
+      <c r="J13" s="56"/>
+      <c r="K13" s="52">
+        <f t="shared" si="1"/>
+        <v>690000</v>
+      </c>
+      <c r="L13" s="46">
+        <v>2</v>
+      </c>
+      <c r="M13" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="N13" s="55">
+        <f t="shared" si="2"/>
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="46">
+        <v>6</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="45">
+        <v>1</v>
+      </c>
+      <c r="F14" s="46">
+        <v>3</v>
+      </c>
+      <c r="G14" s="58">
+        <v>180000</v>
+      </c>
+      <c r="H14" s="53">
+        <f t="shared" si="3"/>
+        <v>540000</v>
+      </c>
+      <c r="I14" s="51">
+        <v>150000</v>
+      </c>
+      <c r="J14" s="59"/>
+      <c r="K14" s="52">
+        <f t="shared" si="1"/>
+        <v>690000</v>
+      </c>
+      <c r="L14" s="46">
+        <v>2</v>
+      </c>
+      <c r="M14" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="N14" s="55">
+        <f t="shared" si="2"/>
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="46">
+        <v>7</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="45">
+        <v>1</v>
+      </c>
+      <c r="F15" s="46">
+        <v>3</v>
+      </c>
+      <c r="G15" s="58">
+        <v>180000</v>
+      </c>
+      <c r="H15" s="53">
+        <f t="shared" si="3"/>
+        <v>540000</v>
+      </c>
+      <c r="I15" s="51">
+        <v>150000</v>
+      </c>
+      <c r="J15" s="56"/>
+      <c r="K15" s="52">
+        <f t="shared" si="1"/>
+        <v>690000</v>
+      </c>
+      <c r="L15" s="46">
+        <v>2</v>
+      </c>
+      <c r="M15" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="N15" s="55">
+        <f t="shared" si="2"/>
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="46">
+        <v>8</v>
+      </c>
+      <c r="B16" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="45">
+        <v>1</v>
+      </c>
+      <c r="F16" s="46">
+        <v>3</v>
+      </c>
+      <c r="G16" s="58">
+        <v>180000</v>
+      </c>
+      <c r="H16" s="53">
+        <f t="shared" si="3"/>
+        <v>540000</v>
+      </c>
+      <c r="I16" s="55"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="52">
+        <f t="shared" si="1"/>
+        <v>540000</v>
+      </c>
+      <c r="L16" s="46">
+        <v>2</v>
+      </c>
+      <c r="M16" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="N16" s="55">
+        <f t="shared" si="2"/>
+        <v>2000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="46">
+        <v>9</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="45">
+        <v>5</v>
+      </c>
+      <c r="F17" s="46">
+        <v>3</v>
+      </c>
+      <c r="G17" s="58">
+        <v>180000</v>
+      </c>
+      <c r="H17" s="53">
+        <f t="shared" si="3"/>
+        <v>540000</v>
+      </c>
+      <c r="I17" s="51">
+        <v>150000</v>
+      </c>
+      <c r="J17" s="56"/>
+      <c r="K17" s="52">
+        <f t="shared" si="1"/>
+        <v>3450000</v>
+      </c>
+      <c r="L17" s="46">
+        <v>2</v>
+      </c>
+      <c r="M17" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="N17" s="55">
+        <f t="shared" si="2"/>
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="46">
+        <v>10</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="45">
+        <v>4</v>
+      </c>
+      <c r="F18" s="46">
+        <v>3</v>
+      </c>
+      <c r="G18" s="58">
+        <v>180000</v>
+      </c>
+      <c r="H18" s="53">
+        <f t="shared" si="3"/>
+        <v>540000</v>
+      </c>
+      <c r="I18" s="51"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="52">
+        <f t="shared" si="1"/>
+        <v>2160000</v>
+      </c>
+      <c r="L18" s="46">
+        <v>2</v>
+      </c>
+      <c r="M18" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="N18" s="55">
+        <f t="shared" si="2"/>
+        <v>8000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="46">
+        <v>11</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="45">
+        <v>8</v>
+      </c>
+      <c r="F19" s="46">
+        <v>3</v>
+      </c>
+      <c r="G19" s="58">
+        <v>180000</v>
+      </c>
+      <c r="H19" s="53">
+        <f t="shared" si="3"/>
+        <v>540000</v>
+      </c>
+      <c r="I19" s="51">
+        <v>150000</v>
+      </c>
+      <c r="J19" s="56"/>
+      <c r="K19" s="52">
+        <f t="shared" si="1"/>
+        <v>5520000</v>
+      </c>
+      <c r="L19" s="46">
+        <v>2</v>
+      </c>
+      <c r="M19" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="N19" s="55">
+        <f t="shared" si="2"/>
+        <v>16000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="46">
+        <v>12</v>
+      </c>
+      <c r="B20" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="45">
+        <v>7</v>
+      </c>
+      <c r="F20" s="46">
+        <v>3</v>
+      </c>
+      <c r="G20" s="58">
+        <v>180000</v>
+      </c>
+      <c r="H20" s="53">
+        <f t="shared" si="3"/>
+        <v>540000</v>
+      </c>
+      <c r="I20" s="51">
+        <v>150000</v>
+      </c>
+      <c r="J20" s="56"/>
+      <c r="K20" s="52">
+        <f t="shared" si="1"/>
+        <v>4830000</v>
+      </c>
+      <c r="L20" s="46">
+        <v>2</v>
+      </c>
+      <c r="M20" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="N20" s="55">
+        <f t="shared" si="2"/>
+        <v>14000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="46">
+        <v>13</v>
+      </c>
+      <c r="B21" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="45">
+        <v>3</v>
+      </c>
+      <c r="F21" s="46">
+        <v>3</v>
+      </c>
+      <c r="G21" s="58">
+        <v>180000</v>
+      </c>
+      <c r="H21" s="53">
+        <f t="shared" si="3"/>
+        <v>540000</v>
+      </c>
+      <c r="I21" s="51">
+        <v>150000</v>
+      </c>
+      <c r="J21" s="56"/>
+      <c r="K21" s="52">
+        <f t="shared" si="1"/>
+        <v>2070000</v>
+      </c>
+      <c r="L21" s="46">
+        <v>2</v>
+      </c>
+      <c r="M21" s="30">
+        <v>1000000</v>
+      </c>
+      <c r="N21" s="55">
+        <f t="shared" si="2"/>
+        <v>6000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="46"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="60">
+        <f>SUM(E9:E21)</f>
+        <v>35</v>
+      </c>
+      <c r="F22" s="46"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="60">
+        <f>SUM(K9:K21)</f>
+        <v>27379000</v>
+      </c>
+      <c r="L22" s="46"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="60">
+        <f>SUM(N9:N21)</f>
+        <v>70000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="97" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="97"/>
+      <c r="C23" s="97"/>
+      <c r="D23" s="97"/>
+      <c r="E23" s="97"/>
+      <c r="F23" s="97"/>
+      <c r="G23" s="97"/>
+      <c r="H23" s="97"/>
+      <c r="I23" s="97"/>
+      <c r="J23" s="97"/>
+      <c r="K23" s="98">
+        <f>K22/E22</f>
+        <v>782257.14285714284</v>
+      </c>
+      <c r="L23" s="97"/>
+      <c r="M23" s="97"/>
+      <c r="N23" s="97"/>
+    </row>
+    <row r="24" spans="1:14" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="64"/>
+      <c r="K24" s="65"/>
+    </row>
+    <row r="25" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="66"/>
+      <c r="H25" s="67"/>
+      <c r="K25" s="65"/>
+    </row>
+    <row r="26" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="66"/>
+      <c r="K26" s="65"/>
+    </row>
+    <row r="27" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="65"/>
+    </row>
+    <row r="28" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="65"/>
+      <c r="K28" s="65"/>
+    </row>
+    <row r="29" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="66"/>
+    </row>
+    <row r="30" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="66"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="70"/>
+    </row>
+    <row r="31" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E31" s="66"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="66"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="70"/>
+      <c r="N32" s="71"/>
+    </row>
+    <row r="33" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="66"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="70"/>
+      <c r="H33" s="70"/>
+      <c r="N33" s="71"/>
+    </row>
+    <row r="34" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E34" s="66"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
+    </row>
+    <row r="35" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="66"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
+    </row>
+    <row r="36" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E36" s="66"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="70"/>
+    </row>
+    <row r="37" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E37" s="66"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
+    </row>
+    <row r="38" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E38" s="66"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="70"/>
+    </row>
+    <row r="39" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E39" s="66"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="68"/>
+    </row>
+    <row r="40" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E40" s="66"/>
+      <c r="F40" s="70"/>
+      <c r="G40" s="70"/>
+      <c r="H40" s="70"/>
+    </row>
+    <row r="41" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E41" s="66"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="70"/>
+    </row>
+    <row r="42" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E42" s="66"/>
+      <c r="F42" s="70"/>
+      <c r="G42" s="70"/>
+      <c r="H42" s="70"/>
+    </row>
+    <row r="43" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E43" s="66"/>
+      <c r="F43" s="70"/>
+      <c r="G43" s="70"/>
+      <c r="H43" s="70"/>
+    </row>
+    <row r="44" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E44" s="66"/>
+      <c r="F44" s="70"/>
+      <c r="G44" s="70"/>
+      <c r="H44" s="70"/>
+    </row>
+    <row r="45" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E45" s="66"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="70"/>
+      <c r="H45" s="70"/>
+    </row>
+    <row r="46" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E46" s="66"/>
+    </row>
+    <row r="47" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E47" s="66"/>
+    </row>
+    <row r="48" spans="5:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E48" s="66"/>
+    </row>
+    <row r="49" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E49" s="66"/>
+    </row>
+    <row r="50" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E50" s="66"/>
+    </row>
+    <row r="51" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E51" s="66"/>
+    </row>
+    <row r="52" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E52" s="66"/>
+    </row>
+    <row r="53" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E53" s="66"/>
+    </row>
+    <row r="54" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E54" s="66"/>
+    </row>
+    <row r="55" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E55" s="66"/>
+    </row>
+    <row r="56" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E56" s="66"/>
+    </row>
+    <row r="57" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E57" s="66"/>
+    </row>
+    <row r="58" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E58" s="66"/>
+    </row>
+    <row r="59" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E59" s="66"/>
+    </row>
+    <row r="60" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E60" s="66"/>
+    </row>
+    <row r="61" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E61" s="66"/>
+    </row>
+    <row r="62" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E62" s="66"/>
+    </row>
+    <row r="63" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E63" s="66"/>
+    </row>
+    <row r="64" spans="5:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E64" s="66"/>
+    </row>
+    <row r="65" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E65" s="66"/>
+    </row>
+    <row r="66" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E66" s="66"/>
+    </row>
+    <row r="67" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E67" s="66"/>
+    </row>
+    <row r="68" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E68" s="66"/>
+    </row>
+    <row r="69" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E69" s="66"/>
+    </row>
+    <row r="70" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E70" s="66"/>
+    </row>
+    <row r="71" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E71" s="66"/>
+    </row>
+    <row r="72" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E72" s="66"/>
+    </row>
+    <row r="73" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E73" s="66"/>
+    </row>
+    <row r="74" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E74" s="66"/>
+    </row>
+    <row r="75" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E75" s="66"/>
+    </row>
+    <row r="76" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E76" s="66"/>
+    </row>
+    <row r="77" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E77" s="66"/>
+    </row>
+    <row r="78" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E78" s="66"/>
+    </row>
+    <row r="79" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E79" s="66"/>
+    </row>
+    <row r="80" spans="1:14" s="72" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="35"/>
+      <c r="B80" s="35"/>
+      <c r="C80" s="35"/>
+      <c r="D80" s="35"/>
+      <c r="E80" s="66"/>
+      <c r="F80" s="35"/>
+      <c r="G80" s="35"/>
+      <c r="H80" s="35"/>
+      <c r="I80" s="35"/>
+      <c r="J80" s="35"/>
+      <c r="K80" s="35"/>
+      <c r="L80" s="35"/>
+      <c r="M80" s="35"/>
+      <c r="N80" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A6:N6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:H7"/>
+  </mergeCells>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>